<commit_message>
Database afgerond en onwikkelomgeving
</commit_message>
<xml_diff>
--- a/Database normaliseren.xlsx
+++ b/Database normaliseren.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Teun\School\MED Leerjaar 2 Periode_05\Project\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Teun\Documents\GitHub\Groep1-Barroc-it\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="143" uniqueCount="99">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="145" uniqueCount="99">
   <si>
     <t xml:space="preserve">CustomerID </t>
   </si>
@@ -404,7 +404,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -415,6 +415,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standaard" xfId="0" builtinId="0"/>
@@ -723,10 +724,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:L53"/>
+  <dimension ref="A2:J53"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="F26" sqref="F26"/>
+      <selection activeCell="E35" sqref="E35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -741,12 +742,8 @@
     <col min="8" max="28" width="30.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="J2" s="7" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="3" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="4" t="s">
         <v>0</v>
       </c>
@@ -759,11 +756,8 @@
       <c r="H3" s="6" t="s">
         <v>52</v>
       </c>
-      <c r="J3" s="6" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
         <v>1</v>
       </c>
@@ -776,11 +770,8 @@
       <c r="H4" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="J4" s="2" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>2</v>
       </c>
@@ -793,11 +784,8 @@
       <c r="H5" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="J5" s="1" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>3</v>
       </c>
@@ -810,11 +798,8 @@
       <c r="H6" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="J6" s="1" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>4</v>
       </c>
@@ -828,7 +813,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>5</v>
       </c>
@@ -842,7 +827,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>6</v>
       </c>
@@ -856,7 +841,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>7</v>
       </c>
@@ -870,7 +855,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>8</v>
       </c>
@@ -882,7 +867,7 @@
       </c>
       <c r="H11" s="1"/>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>9</v>
       </c>
@@ -890,7 +875,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>10</v>
       </c>
@@ -898,7 +883,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>11</v>
       </c>
@@ -906,7 +891,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>12</v>
       </c>
@@ -914,7 +899,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>13</v>
       </c>
@@ -922,7 +907,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>14</v>
       </c>
@@ -931,7 +916,7 @@
       </c>
       <c r="F17" s="9"/>
     </row>
-    <row r="18" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>15</v>
       </c>
@@ -939,8 +924,9 @@
         <v>59</v>
       </c>
       <c r="F18" s="9"/>
-    </row>
-    <row r="19" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="H18" s="7"/>
+    </row>
+    <row r="19" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>16</v>
       </c>
@@ -953,14 +939,8 @@
       <c r="H19" s="6" t="s">
         <v>90</v>
       </c>
-      <c r="J19" s="6" t="s">
-        <v>91</v>
-      </c>
-      <c r="L19" s="6" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>17</v>
       </c>
@@ -973,34 +953,22 @@
       <c r="H20" s="2" t="s">
         <v>93</v>
       </c>
-      <c r="J20" s="8" t="s">
-        <v>93</v>
-      </c>
-      <c r="L20" s="2" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="21" spans="1:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>18</v>
       </c>
       <c r="D21" s="3" t="s">
         <v>97</v>
       </c>
-      <c r="F21" s="1" t="s">
-        <v>67</v>
+      <c r="F21" s="2" t="s">
+        <v>93</v>
       </c>
       <c r="H21" t="s">
         <v>69</v>
       </c>
-      <c r="J21" s="8" t="s">
-        <v>94</v>
-      </c>
-      <c r="L21" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="22" spans="1:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>19</v>
       </c>
@@ -1013,38 +981,34 @@
       <c r="H22" t="s">
         <v>65</v>
       </c>
-      <c r="J22" s="9"/>
-      <c r="L22" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="23" spans="1:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>20</v>
       </c>
       <c r="F23" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="J23" s="9"/>
-    </row>
-    <row r="24" spans="1:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>21</v>
       </c>
+      <c r="F24" s="10"/>
       <c r="J24" s="9"/>
     </row>
-    <row r="25" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>22</v>
       </c>
       <c r="J25" s="9"/>
     </row>
-    <row r="26" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="27" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>24</v>
       </c>
@@ -1052,7 +1016,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="28" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>25</v>
       </c>
@@ -1060,7 +1024,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>26</v>
       </c>
@@ -1068,7 +1032,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="30" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>27</v>
       </c>
@@ -1076,7 +1040,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="31" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>28</v>
       </c>
@@ -1084,7 +1048,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="32" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>29</v>
       </c>
@@ -1215,21 +1179,25 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:C34"/>
+  <dimension ref="A2:M34"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C35" sqref="C35"/>
+      <selection activeCell="L10" sqref="L10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="11" max="11" width="21.7109375" customWidth="1"/>
+    <col min="13" max="13" width="21.7109375" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" s="9"/>
       <c r="B2" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="9" t="s">
         <v>67</v>
       </c>
@@ -1239,29 +1207,48 @@
       <c r="C3" t="s">
         <v>65</v>
       </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="K3" s="7" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B4" t="s">
         <v>71</v>
       </c>
       <c r="C4" t="s">
         <v>72</v>
       </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="K4" s="6" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
         <v>73</v>
       </c>
       <c r="C5" t="s">
         <v>74</v>
       </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="K5" s="2" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="K6" s="1" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="K7" s="1" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B8" s="7" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>80</v>
       </c>
@@ -1272,7 +1259,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B10" s="1" t="s">
         <v>75</v>
       </c>
@@ -1280,27 +1267,27 @@
         <v>76</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B11" s="1" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B12" s="1" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B13" s="1" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B15" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B16" t="s">
         <v>67</v>
       </c>
@@ -1308,7 +1295,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B17">
         <v>1</v>
       </c>
@@ -1316,7 +1303,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B18">
         <v>1</v>
       </c>
@@ -1324,51 +1311,84 @@
         <v>2</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B19">
         <v>1</v>
       </c>
       <c r="C19">
         <v>3</v>
       </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="K19" s="7" t="s">
+        <v>96</v>
+      </c>
+      <c r="M19" s="7" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="20" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B20">
         <v>1</v>
       </c>
       <c r="C20">
         <v>4</v>
       </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="K20" s="6" t="s">
+        <v>91</v>
+      </c>
+      <c r="M20" s="6" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="21" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B21">
         <v>2</v>
       </c>
       <c r="C21">
         <v>2</v>
       </c>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="K21" s="8" t="s">
+        <v>93</v>
+      </c>
+      <c r="M21" s="2" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="22" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B22">
         <v>3</v>
       </c>
-    </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="K22" s="8" t="s">
+        <v>94</v>
+      </c>
+      <c r="M22" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="23" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="K23" s="9"/>
+      <c r="M23" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="24" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="K24" s="9"/>
+    </row>
+    <row r="26" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>85</v>
       </c>

</xml_diff>